<commit_message>
Kfin support and improvements
</commit_message>
<xml_diff>
--- a/MF_Summary.xlsx
+++ b/MF_Summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Fund</t>
   </si>
@@ -40,13 +40,34 @@
     <t>XIRR - Nifty Equiv.</t>
   </si>
   <si>
-    <t>AXIS BLUECHIP FUND - DIRECT PLAN</t>
-  </si>
-  <si>
-    <t>ICICI PRUDENTIAL NIFTY INDEX FUND - DIRECT PLAN</t>
-  </si>
-  <si>
-    <t>SBI FOCUSED EQUITY FUND - DIRECT PLAN</t>
+    <t>HDFC Balanced Advantage Fund Direct Plan Growth</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Nifty 50 Index Direct Plan Growth</t>
+  </si>
+  <si>
+    <t>Kotak Emerging Equity Fund Direct Growth</t>
+  </si>
+  <si>
+    <t>Parag Parikh Flexi Cap Fund Direct Growth</t>
+  </si>
+  <si>
+    <t>SBI Bluechip Direct Plan Growth</t>
+  </si>
+  <si>
+    <t>SBI Small Cap Fund Direct Growth</t>
+  </si>
+  <si>
+    <t>Mirae Asset Emerging Bluechip Fund - Direct Plan Growth</t>
+  </si>
+  <si>
+    <t>Axis Mid Cap Fund - Direct Growth</t>
+  </si>
+  <si>
+    <t>NIPPON INDIA SMALL CAP FUND - DIRECT GROWTH PLAN GROWTH OPTION</t>
+  </si>
+  <si>
+    <t>Overall</t>
   </si>
 </sst>
 </file>
@@ -404,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,25 +462,25 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>8509.5</v>
+        <v>2999.574</v>
       </c>
       <c r="C2">
-        <v>7656</v>
+        <v>3132.127</v>
       </c>
       <c r="D2">
-        <v>357.39</v>
+        <v>44.298</v>
       </c>
       <c r="E2">
-        <v>-10.03</v>
+        <v>4.419</v>
       </c>
       <c r="F2">
-        <v>-1.017</v>
+        <v>2.205</v>
       </c>
       <c r="G2">
-        <v>-10.232</v>
+        <v>42.302</v>
       </c>
       <c r="H2">
-        <v>-1.039</v>
+        <v>19.578</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -467,25 +488,25 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>20107.944</v>
+        <v>3999.799</v>
       </c>
       <c r="C3">
-        <v>20093.843</v>
+        <v>4055.674</v>
       </c>
       <c r="D3">
-        <v>353.838</v>
+        <v>58.501</v>
       </c>
       <c r="E3">
-        <v>-0.07000000000000001</v>
+        <v>1.397</v>
       </c>
       <c r="F3">
-        <v>-1.076</v>
+        <v>1.044</v>
       </c>
       <c r="G3">
-        <v>-0.07199999999999999</v>
+        <v>9.023999999999999</v>
       </c>
       <c r="H3">
-        <v>-1.11</v>
+        <v>6.688</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -493,25 +514,207 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>20572.28</v>
+        <v>2999.846</v>
       </c>
       <c r="C4">
-        <v>19892.32</v>
+        <v>3113.145</v>
       </c>
       <c r="D4">
+        <v>34.667</v>
+      </c>
+      <c r="E4">
+        <v>3.777</v>
+      </c>
+      <c r="F4">
+        <v>0.338</v>
+      </c>
+      <c r="G4">
+        <v>47.207</v>
+      </c>
+      <c r="H4">
+        <v>3.617</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>3999.803</v>
+      </c>
+      <c r="C5">
+        <v>4031.681</v>
+      </c>
+      <c r="D5">
+        <v>40.5</v>
+      </c>
+      <c r="E5">
+        <v>0.797</v>
+      </c>
+      <c r="F5">
+        <v>1.147</v>
+      </c>
+      <c r="G5">
+        <v>7.399</v>
+      </c>
+      <c r="H5">
+        <v>10.786</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>3999.815</v>
+      </c>
+      <c r="C6">
+        <v>3952.529</v>
+      </c>
+      <c r="D6">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>-1.182</v>
+      </c>
+      <c r="F6">
+        <v>-0.998</v>
+      </c>
+      <c r="G6">
+        <v>-16.576</v>
+      </c>
+      <c r="H6">
+        <v>-14.177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>1999.897</v>
+      </c>
+      <c r="C7">
+        <v>2032.165</v>
+      </c>
+      <c r="D7">
+        <v>19.5</v>
+      </c>
+      <c r="E7">
+        <v>1.613</v>
+      </c>
+      <c r="F7">
+        <v>-0.97</v>
+      </c>
+      <c r="G7">
+        <v>34.73</v>
+      </c>
+      <c r="H7">
+        <v>-16.726</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>1999.843</v>
+      </c>
+      <c r="C8">
+        <v>2020.721</v>
+      </c>
+      <c r="D8">
         <v>28</v>
       </c>
-      <c r="E4">
-        <v>-3.305</v>
-      </c>
-      <c r="F4">
-        <v>-3.445</v>
-      </c>
-      <c r="G4">
-        <v>-35.477</v>
-      </c>
-      <c r="H4">
-        <v>-36.679</v>
+      <c r="E8">
+        <v>1.044</v>
+      </c>
+      <c r="F8">
+        <v>-2.202</v>
+      </c>
+      <c r="G8">
+        <v>14.498</v>
+      </c>
+      <c r="H8">
+        <v>-25.196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>999.944</v>
+      </c>
+      <c r="C9">
+        <v>1005.537</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>0.5590000000000001</v>
+      </c>
+      <c r="F9">
+        <v>-1.841</v>
+      </c>
+      <c r="G9">
+        <v>8.484999999999999</v>
+      </c>
+      <c r="H9">
+        <v>-23.762</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>999.8920000000001</v>
+      </c>
+      <c r="C10">
+        <v>1021.12</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>2.123</v>
+      </c>
+      <c r="F10">
+        <v>-1.841</v>
+      </c>
+      <c r="G10">
+        <v>35.896</v>
+      </c>
+      <c r="H10">
+        <v>-23.762</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>23998.412</v>
+      </c>
+      <c r="C11">
+        <v>24364.7</v>
+      </c>
+      <c r="D11">
+        <v>36.412</v>
+      </c>
+      <c r="E11">
+        <v>1.526</v>
+      </c>
+      <c r="F11">
+        <v>0.099</v>
+      </c>
+      <c r="G11">
+        <v>16.327</v>
+      </c>
+      <c r="H11">
+        <v>0.995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>